<commit_message>
Add Stage 2 - dummy script
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage2/2-1 npc.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage2/2-1 npc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uisoo/Documents/GitHub/Project-Caterpillar/Assets/Editor/JsonUtility/JsonUtility/Stage2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D2CED8-9721-DC4C-B77E-76F8DD6CF2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAC94A-0F80-4FAB-AA33-B4A5C38B9172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15640" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -3135,10 +3135,6 @@
     <t>비만</t>
   </si>
   <si>
-    <t>Hold, -1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>골목대장</t>
   </si>
   <si>
@@ -3168,6 +3164,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···!</t>
     </r>
@@ -3199,6 +3197,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">···! </t>
     </r>
@@ -3217,6 +3217,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3235,6 +3237,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.)</t>
     </r>
@@ -3248,6 +3252,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3274,6 +3280,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.</t>
     </r>
@@ -3302,6 +3310,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.</t>
     </r>
@@ -3384,6 +3394,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···!</t>
     </r>
@@ -3430,6 +3442,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3481,6 +3495,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3568,6 +3584,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3586,6 +3604,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3604,6 +3624,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.</t>
     </r>
@@ -3627,6 +3649,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3656,6 +3680,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3739,6 +3765,22 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hold, -1, name=Stage 2/2-1/Remove </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개척자</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -3811,6 +3853,8 @@
       <sz val="9"/>
       <color rgb="FFA6A6A6"/>
       <name val="A고딕12"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3819,9 +3863,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="A고딕12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4088,9 +4134,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -5170,24 +5216,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -5250,7 +5296,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5264,7 +5310,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5276,7 +5322,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5383,20 +5429,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
@@ -5461,10 +5507,10 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -5474,10 +5520,10 @@
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -5486,10 +5532,10 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -5509,10 +5555,10 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5520,10 +5566,10 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -5542,10 +5588,10 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -5553,10 +5599,10 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -5564,10 +5610,10 @@
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6581,20 +6627,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6664,10 +6710,10 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -6689,10 +6735,10 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -6713,10 +6759,10 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -6724,7 +6770,7 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>21</v>
@@ -6736,10 +6782,10 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -6748,10 +6794,10 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -6759,7 +6805,7 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
@@ -6781,10 +6827,10 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -7794,23 +7840,23 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="130.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="130.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7883,7 +7929,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -7896,7 +7942,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -7907,7 +7953,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -7919,7 +7965,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -7942,7 +7988,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -7953,7 +7999,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -7964,7 +8010,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -7975,7 +8021,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -7997,7 +8043,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -8008,7 +8054,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -8024,16 +8070,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="16.5">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
@@ -9033,19 +9079,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9118,7 +9164,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9129,7 +9175,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -9141,7 +9187,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -9152,7 +9198,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9163,7 +9209,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -9192,19 +9238,19 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9274,10 +9320,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -9291,7 +9337,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -9299,10 +9345,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -9314,7 +9360,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9322,10 +9368,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -9344,10 +9390,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -9355,10 +9401,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -9398,24 +9444,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -9475,10 +9521,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9492,7 +9538,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -9500,10 +9546,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -9512,10 +9558,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9629,24 +9675,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -9709,7 +9755,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9824,24 +9870,24 @@
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -9901,10 +9947,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9918,7 +9964,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6">
         <v>1</v>

</xml_diff>

<commit_message>
Add Stage 2 - dummy script (#122)
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage2/2-1 npc.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage2/2-1 npc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uisoo/Documents/GitHub/Project-Caterpillar/Assets/Editor/JsonUtility/JsonUtility/Stage2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D2CED8-9721-DC4C-B77E-76F8DD6CF2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CAC94A-0F80-4FAB-AA33-B4A5C38B9172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15640" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -3135,10 +3135,6 @@
     <t>비만</t>
   </si>
   <si>
-    <t>Hold, -1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>골목대장</t>
   </si>
   <si>
@@ -3168,6 +3164,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···!</t>
     </r>
@@ -3199,6 +3197,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">···! </t>
     </r>
@@ -3217,6 +3217,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3235,6 +3237,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.)</t>
     </r>
@@ -3248,6 +3252,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3274,6 +3280,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.</t>
     </r>
@@ -3302,6 +3310,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.</t>
     </r>
@@ -3384,6 +3394,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···!</t>
     </r>
@@ -3430,6 +3442,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3481,6 +3495,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3568,6 +3584,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3586,6 +3604,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3604,6 +3624,8 @@
         <sz val="9"/>
         <color rgb="FFA6A6A6"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···.</t>
     </r>
@@ -3627,6 +3649,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>···</t>
     </r>
@@ -3656,6 +3680,8 @@
         <sz val="9"/>
         <color rgb="FF000000"/>
         <rFont val="A고딕12"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t xml:space="preserve">··· </t>
     </r>
@@ -3739,6 +3765,22 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hold, -1, name=Stage 2/2-1/Remove </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개척자</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -3811,6 +3853,8 @@
       <sz val="9"/>
       <color rgb="FFA6A6A6"/>
       <name val="A고딕12"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3819,9 +3863,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="A고딕12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4088,9 +4134,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.83203125" customWidth="1"/>
+    <col min="1" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -5170,24 +5216,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -5250,7 +5296,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -5264,7 +5310,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -5276,7 +5322,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -5383,20 +5429,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
@@ -5461,10 +5507,10 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -5474,10 +5520,10 @@
     </row>
     <row r="6" spans="1:6" ht="16.5" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -5486,10 +5532,10 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -5509,10 +5555,10 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5520,10 +5566,10 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -5542,10 +5588,10 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -5553,10 +5599,10 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -5564,10 +5610,10 @@
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -6581,20 +6627,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" customWidth="1"/>
-    <col min="2" max="2" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -6664,10 +6710,10 @@
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -6689,10 +6735,10 @@
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -6713,10 +6759,10 @@
     </row>
     <row r="9" spans="1:6" ht="16.5" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -6724,7 +6770,7 @@
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>21</v>
@@ -6736,10 +6782,10 @@
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -6748,10 +6794,10 @@
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -6759,7 +6805,7 @@
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>18</v>
@@ -6781,10 +6827,10 @@
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -7794,23 +7840,23 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="130.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="130.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -7883,7 +7929,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -7896,7 +7942,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -7907,7 +7953,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -7919,7 +7965,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -7942,7 +7988,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -7953,7 +7999,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -7964,7 +8010,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -7975,7 +8021,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -7997,7 +8043,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -8008,7 +8054,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -8024,16 +8070,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" ht="16.5">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" customHeight="1"/>
@@ -9033,19 +9079,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9118,7 +9164,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9129,7 +9175,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -9141,7 +9187,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -9152,7 +9198,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9163,7 +9209,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -9192,19 +9238,19 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9274,10 +9320,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -9291,7 +9337,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -9299,10 +9345,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -9314,7 +9360,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9322,10 +9368,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -9344,10 +9390,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -9355,10 +9401,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -9398,24 +9444,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -9475,10 +9521,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9492,7 +9538,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -9500,10 +9546,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -9512,10 +9558,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -9629,24 +9675,24 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -9709,7 +9755,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9824,24 +9870,24 @@
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17">
+    <row r="1" spans="1:6" ht="16.5">
       <c r="A1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -9901,10 +9947,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -9918,7 +9964,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6">
         <v>1</v>

</xml_diff>